<commit_message>
Add Elements of Schooling, Reportale Subjects, Skills and Completion tabs Modified ReadWriteDataToExcel to return int instead of String Modified TC003, TC004 Add more actions on TC005 Add fileUpload.txt
</commit_message>
<xml_diff>
--- a/src/Data.xlsx
+++ b/src/Data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace\MinistryOfEducation\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="7310" windowWidth="19200" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sponsor" r:id="rId1" sheetId="1"/>
-    <sheet name="Client" r:id="rId2" sheetId="2"/>
+    <sheet name="Sponsor" sheetId="1" r:id="rId1"/>
+    <sheet name="Client" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,19 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>2948455</t>
-  </si>
-  <si>
-    <t>2948456</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -65,16 +57,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -91,10 +83,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -129,7 +121,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -164,7 +156,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,21 +250,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -289,7 +281,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -341,48 +333,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add updateDB method to TC005 Completed TC008, RC009
</commit_message>
<xml_diff>
--- a/src/Data.xlsx
+++ b/src/Data.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse-workspace\MinistryOfEducation\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" activeTab="1"/>
+    <workbookView windowHeight="7310" windowWidth="19200" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sponsor" sheetId="1" r:id="rId1"/>
-    <sheet name="Client" sheetId="2" r:id="rId2"/>
+    <sheet name="Sponsor" r:id="rId1" sheetId="1"/>
+    <sheet name="Client" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,11 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -57,16 +58,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -83,10 +84,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -121,7 +122,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -156,7 +157,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,21 +251,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -281,7 +282,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -333,36 +334,68 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>2948492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2948532</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2948534</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>2948512</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2948533</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2948535.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>